<commit_message>
Update of mark-1 workbench visio
Updated the mark-1 workbench visio to show the relationship between the excel fields and the individual data graphics.  Also modified the spreadsheet to hide unused columns for each data graphic, and push also grabbed a few updates in the icon repository
</commit_message>
<xml_diff>
--- a/DG-stencil-sets/mark-1/workbench/mark-1-data-graphic-input.xlsx
+++ b/DG-stencil-sets/mark-1/workbench/mark-1-data-graphic-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/ken_rollins_emc_com/Documents/Projects/TechProfile/DG-stencil-sets/mark-1/workbench/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="13_ncr:1_{FA68AA0A-2D18-4051-9A7E-52C5C09362B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BD04C701-6690-44F5-843E-252E8D5DF978}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="13_ncr:1_{FA68AA0A-2D18-4051-9A7E-52C5C09362B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F22C1D04-30E0-44FD-8CC6-41FE321F7BF6}"/>
   <bookViews>
-    <workbookView xWindow="1657" yWindow="638" windowWidth="25591" windowHeight="13612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="473" yWindow="2588" windowWidth="27900" windowHeight="8257" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -1158,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
@@ -2391,7 +2391,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2402,7 +2402,7 @@
     <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" customWidth="1"/>
     <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
+    <col min="8" max="8" width="19.46484375" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.9296875" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
@@ -3346,10 +3346,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC73515-619F-49CB-A260-4515E2B5E74C}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3357,10 +3357,10 @@
     <col min="1" max="1" width="7.9296875" customWidth="1"/>
     <col min="2" max="3" width="20.19921875" customWidth="1"/>
     <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.9296875" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
@@ -4279,7 +4279,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4287,11 +4287,11 @@
     <col min="1" max="1" width="7.9296875" customWidth="1"/>
     <col min="2" max="3" width="20.19921875" customWidth="1"/>
     <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
   </cols>
@@ -5191,9 +5191,9 @@
   <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5201,11 +5201,11 @@
     <col min="1" max="1" width="7.9296875" customWidth="1"/>
     <col min="2" max="3" width="20.19921875" customWidth="1"/>
     <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
   </cols>
@@ -6209,9 +6209,9 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6219,11 +6219,11 @@
     <col min="1" max="1" width="7.9296875" customWidth="1"/>
     <col min="2" max="3" width="20.19921875" customWidth="1"/>
     <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
   </cols>
@@ -6820,7 +6820,7 @@
         <v>73</v>
       </c>
       <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="20"/>
       <c r="F35" s="25"/>
       <c r="G35" s="14"/>
@@ -6836,7 +6836,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="20"/>
       <c r="F36" s="25"/>
       <c r="G36" s="14"/>
@@ -6852,7 +6852,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="25"/>
-      <c r="D37" s="26"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="20"/>
       <c r="F37" s="25"/>
       <c r="G37" s="14"/>
@@ -6868,7 +6868,7 @@
         <v>73</v>
       </c>
       <c r="C38" s="25"/>
-      <c r="D38" s="26"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="20"/>
       <c r="F38" s="25"/>
       <c r="G38" s="14"/>
@@ -6884,7 +6884,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="25"/>
-      <c r="D39" s="26"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="20"/>
       <c r="F39" s="25"/>
       <c r="G39" s="14"/>
@@ -6900,7 +6900,7 @@
         <v>73</v>
       </c>
       <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="20"/>
       <c r="F40" s="25"/>
       <c r="G40" s="14"/>
@@ -6916,7 +6916,7 @@
         <v>73</v>
       </c>
       <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="20"/>
       <c r="F41" s="25"/>
       <c r="G41" s="14"/>
@@ -6932,7 +6932,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="20"/>
       <c r="F42" s="25"/>
       <c r="G42" s="14"/>
@@ -6948,7 +6948,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="20"/>
       <c r="F43" s="25"/>
       <c r="G43" s="14"/>
@@ -6964,7 +6964,7 @@
         <v>73</v>
       </c>
       <c r="C44" s="25"/>
-      <c r="D44" s="26"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="20"/>
       <c r="F44" s="25"/>
       <c r="G44" s="14"/>
@@ -6980,7 +6980,7 @@
         <v>73</v>
       </c>
       <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="20"/>
       <c r="F45" s="25"/>
       <c r="G45" s="14"/>
@@ -6996,7 +6996,7 @@
         <v>73</v>
       </c>
       <c r="C46" s="25"/>
-      <c r="D46" s="26"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="20"/>
       <c r="F46" s="25"/>
       <c r="G46" s="14"/>
@@ -7012,7 +7012,7 @@
         <v>73</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="20"/>
       <c r="F47" s="25"/>
       <c r="G47" s="14"/>
@@ -7028,7 +7028,7 @@
         <v>73</v>
       </c>
       <c r="C48" s="25"/>
-      <c r="D48" s="26"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="20"/>
       <c r="F48" s="25"/>
       <c r="G48" s="14"/>
@@ -7044,7 +7044,7 @@
         <v>73</v>
       </c>
       <c r="C49" s="25"/>
-      <c r="D49" s="26"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="20"/>
       <c r="F49" s="25"/>
       <c r="G49" s="14"/>
@@ -7060,7 +7060,7 @@
         <v>73</v>
       </c>
       <c r="C50" s="25"/>
-      <c r="D50" s="26"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="20"/>
       <c r="F50" s="25"/>
       <c r="G50" s="14"/>
@@ -7076,7 +7076,7 @@
         <v>73</v>
       </c>
       <c r="C51" s="25"/>
-      <c r="D51" s="26"/>
+      <c r="D51" s="27"/>
       <c r="E51" s="20"/>
       <c r="F51" s="25"/>
       <c r="G51" s="14"/>
@@ -7092,7 +7092,7 @@
         <v>73</v>
       </c>
       <c r="C52" s="25"/>
-      <c r="D52" s="26"/>
+      <c r="D52" s="27"/>
       <c r="E52" s="20"/>
       <c r="F52" s="25"/>
       <c r="G52" s="14"/>
@@ -7108,7 +7108,7 @@
         <v>73</v>
       </c>
       <c r="C53" s="25"/>
-      <c r="D53" s="26"/>
+      <c r="D53" s="27"/>
       <c r="E53" s="20"/>
       <c r="F53" s="25"/>
       <c r="G53" s="14"/>
@@ -7124,7 +7124,7 @@
         <v>73</v>
       </c>
       <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
+      <c r="D54" s="27"/>
       <c r="E54" s="20"/>
       <c r="F54" s="25"/>
       <c r="G54" s="14"/>
@@ -7140,7 +7140,7 @@
         <v>73</v>
       </c>
       <c r="C55" s="25"/>
-      <c r="D55" s="26"/>
+      <c r="D55" s="27"/>
       <c r="E55" s="20"/>
       <c r="F55" s="25"/>
       <c r="G55" s="14"/>
@@ -7156,7 +7156,7 @@
         <v>73</v>
       </c>
       <c r="C56" s="25"/>
-      <c r="D56" s="26"/>
+      <c r="D56" s="27"/>
       <c r="E56" s="20"/>
       <c r="F56" s="25"/>
       <c r="G56" s="14"/>
@@ -7172,7 +7172,7 @@
         <v>73</v>
       </c>
       <c r="C57" s="25"/>
-      <c r="D57" s="26"/>
+      <c r="D57" s="27"/>
       <c r="E57" s="20"/>
       <c r="F57" s="25"/>
       <c r="G57" s="14"/>
@@ -7188,7 +7188,7 @@
         <v>73</v>
       </c>
       <c r="C58" s="25"/>
-      <c r="D58" s="26"/>
+      <c r="D58" s="27"/>
       <c r="E58" s="20"/>
       <c r="F58" s="25"/>
       <c r="G58" s="14"/>
@@ -7204,7 +7204,7 @@
         <v>73</v>
       </c>
       <c r="C59" s="25"/>
-      <c r="D59" s="26"/>
+      <c r="D59" s="27"/>
       <c r="E59" s="20"/>
       <c r="F59" s="25"/>
       <c r="G59" s="14"/>
@@ -7220,7 +7220,7 @@
         <v>73</v>
       </c>
       <c r="C60" s="25"/>
-      <c r="D60" s="26"/>
+      <c r="D60" s="27"/>
       <c r="E60" s="20"/>
       <c r="F60" s="25"/>
       <c r="G60" s="14"/>
@@ -7236,7 +7236,7 @@
         <v>73</v>
       </c>
       <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
+      <c r="D61" s="27"/>
       <c r="E61" s="20"/>
       <c r="F61" s="25"/>
       <c r="G61" s="14"/>
@@ -7261,19 +7261,20 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.796875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="16.19921875" style="36" customWidth="1"/>
     <col min="6" max="6" width="74.33203125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="82.73046875" customWidth="1"/>
     <col min="11" max="11" width="8.73046875" customWidth="1"/>
   </cols>
@@ -7990,6 +7991,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E588E3CCEF65154AAAA5938E9E65CE17" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03844ae5e13aa177ebf3507b0751d91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e85ca4a-4ac1-4389-acba-849333013406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb1ad88d086bd6ffd9f20c44ca8152ce" ns2:_="">
     <xsd:import namespace="0e85ca4a-4ac1-4389-acba-849333013406"/>
@@ -8147,12 +8154,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4776DA57-D8F8-44AA-B808-89F6418CE6E5}">
   <ds:schemaRefs>
@@ -8162,6 +8163,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECED21D3-74F5-44AF-93F1-3A615F6BB7E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD09570-86F7-4181-B0EF-3E1223C67D7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8177,13 +8187,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECED21D3-74F5-44AF-93F1-3A615F6BB7E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Addition of Pre-Linked Visio file to C:\DellEMC\TechProfile directory
Created a prelinked visio and excel file pairing.  The user just needs to copy both files to their local C:\DellEMC\TechProfile directory and they can begin using.
</commit_message>
<xml_diff>
--- a/DG-stencil-sets/mark-1/workbench/mark-1-data-graphic-input.xlsx
+++ b/DG-stencil-sets/mark-1/workbench/mark-1-data-graphic-input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/ken_rollins_emc_com/Documents/Projects/TechProfile/DG-stencil-sets/mark-1/workbench/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="13_ncr:1_{FA68AA0A-2D18-4051-9A7E-52C5C09362B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F22C1D04-30E0-44FD-8CC6-41FE321F7BF6}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{FA68AA0A-2D18-4051-9A7E-52C5C09362B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76EE6C6C-C601-407A-A8D1-6774207FF429}"/>
   <bookViews>
-    <workbookView xWindow="473" yWindow="2588" windowWidth="27900" windowHeight="8257" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17194" yWindow="43" windowWidth="12257" windowHeight="11674" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="191">
   <si>
     <t>Section</t>
   </si>
@@ -601,6 +601,18 @@
   </si>
   <si>
     <t>Operating System</t>
+  </si>
+  <si>
+    <t>CEPH</t>
+  </si>
+  <si>
+    <t>Puppet</t>
+  </si>
+  <si>
+    <t>Slurm</t>
+  </si>
+  <si>
+    <t>Workload manager</t>
   </si>
 </sst>
 </file>
@@ -1158,27 +1170,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="21.59765625" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" customWidth="1"/>
+    <col min="8" max="8" width="21.61328125" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1240,7 +1252,7 @@
       </c>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1270,7 +1282,7 @@
       </c>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1300,7 +1312,7 @@
       </c>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1330,7 +1342,7 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1360,7 +1372,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1390,7 +1402,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1420,7 +1432,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1450,7 +1462,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1480,7 +1492,7 @@
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1510,7 +1522,7 @@
       </c>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1540,7 +1552,7 @@
       </c>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1570,7 +1582,7 @@
       </c>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1600,7 +1612,7 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1630,7 +1642,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1660,7 +1672,7 @@
       </c>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1690,7 +1702,7 @@
       </c>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1720,7 +1732,7 @@
       </c>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1750,7 +1762,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1780,7 +1792,7 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1810,7 +1822,7 @@
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1840,7 +1852,7 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1870,7 +1882,7 @@
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1900,7 +1912,7 @@
       </c>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1930,7 +1942,7 @@
       </c>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1960,7 +1972,7 @@
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1990,23 +2002,37 @@
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2022,7 +2048,7 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2038,7 +2064,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2054,7 +2080,7 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2070,7 +2096,7 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2086,7 +2112,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2102,7 +2128,7 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2118,7 +2144,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2134,7 +2160,7 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2150,7 +2176,7 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2166,7 +2192,7 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2182,7 +2208,7 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2198,7 +2224,7 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2214,7 +2240,7 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2230,7 +2256,7 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2246,7 +2272,7 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2262,7 +2288,7 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2278,7 +2304,7 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2294,7 +2320,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2310,7 +2336,7 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2326,7 +2352,7 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2342,7 +2368,7 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2358,7 +2384,7 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2394,21 +2420,21 @@
       <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" customWidth="1"/>
-    <col min="8" max="8" width="19.46484375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" customWidth="1"/>
+    <col min="8" max="8" width="19.4609375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2440,7 +2466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2468,7 +2494,7 @@
       </c>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2496,7 +2522,7 @@
       </c>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2524,7 +2550,7 @@
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2552,7 +2578,7 @@
       </c>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2580,7 +2606,7 @@
       </c>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2608,7 +2634,7 @@
       </c>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2636,7 +2662,7 @@
       </c>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2664,7 +2690,7 @@
       </c>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2692,7 +2718,7 @@
       </c>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2708,7 +2734,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2724,7 +2750,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2740,7 +2766,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2756,7 +2782,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2772,7 +2798,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2788,7 +2814,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2804,7 +2830,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2820,7 +2846,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2836,7 +2862,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2852,7 +2878,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2868,7 +2894,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2884,7 +2910,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2900,7 +2926,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2916,7 +2942,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="11"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2932,7 +2958,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2948,7 +2974,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2964,7 +2990,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2980,7 +3006,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2996,7 +3022,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3012,7 +3038,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3028,7 +3054,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3044,7 +3070,7 @@
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3060,7 +3086,7 @@
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3076,7 +3102,7 @@
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3092,7 +3118,7 @@
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3108,7 +3134,7 @@
       <c r="I36" s="11"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3124,7 +3150,7 @@
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3140,7 +3166,7 @@
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3156,7 +3182,7 @@
       <c r="I39" s="11"/>
       <c r="J39" s="11"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3172,7 +3198,7 @@
       <c r="I40" s="11"/>
       <c r="J40" s="11"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3188,7 +3214,7 @@
       <c r="I41" s="11"/>
       <c r="J41" s="11"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3204,7 +3230,7 @@
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3220,7 +3246,7 @@
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3236,7 +3262,7 @@
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3252,7 +3278,7 @@
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3268,7 +3294,7 @@
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3284,7 +3310,7 @@
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3300,7 +3326,7 @@
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3316,7 +3342,7 @@
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3352,21 +3378,21 @@
       <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.921875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -3398,7 +3424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3422,7 +3448,7 @@
       </c>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3446,7 +3472,7 @@
       </c>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3470,7 +3496,7 @@
       </c>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3494,7 +3520,7 @@
       </c>
       <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3518,7 +3544,7 @@
       </c>
       <c r="J6" s="15"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3542,7 +3568,7 @@
       </c>
       <c r="J7" s="15"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3566,7 +3592,7 @@
       </c>
       <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3590,7 +3616,7 @@
       </c>
       <c r="J9" s="15"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3614,7 +3640,7 @@
       </c>
       <c r="J10" s="15"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3638,7 +3664,7 @@
       </c>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3654,7 +3680,7 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3670,7 +3696,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3686,7 +3712,7 @@
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3702,7 +3728,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3718,7 +3744,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3734,7 +3760,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3750,7 +3776,7 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3766,7 +3792,7 @@
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3782,7 +3808,7 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3798,7 +3824,7 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3814,7 +3840,7 @@
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3830,7 +3856,7 @@
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3846,7 +3872,7 @@
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3862,7 +3888,7 @@
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3878,7 +3904,7 @@
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3894,7 +3920,7 @@
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3910,7 +3936,7 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3926,7 +3952,7 @@
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3942,7 +3968,7 @@
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3958,7 +3984,7 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3974,7 +4000,7 @@
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3990,7 +4016,7 @@
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -4006,7 +4032,7 @@
       <c r="I34" s="15"/>
       <c r="J34" s="15"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -4022,7 +4048,7 @@
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -4038,7 +4064,7 @@
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4054,7 +4080,7 @@
       <c r="I37" s="15"/>
       <c r="J37" s="15"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4070,7 +4096,7 @@
       <c r="I38" s="15"/>
       <c r="J38" s="15"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4086,7 +4112,7 @@
       <c r="I39" s="15"/>
       <c r="J39" s="15"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4102,7 +4128,7 @@
       <c r="I40" s="15"/>
       <c r="J40" s="15"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4118,7 +4144,7 @@
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4134,7 +4160,7 @@
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4150,7 +4176,7 @@
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4166,7 +4192,7 @@
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4182,7 +4208,7 @@
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4198,7 +4224,7 @@
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4214,7 +4240,7 @@
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4230,7 +4256,7 @@
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4246,7 +4272,7 @@
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4282,21 +4308,21 @@
       <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.921875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -4328,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4350,7 +4376,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="18"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -4370,7 +4396,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -4390,7 +4416,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -4412,7 +4438,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="18"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4434,7 +4460,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="18"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4456,7 +4482,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -4478,7 +4504,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -4500,7 +4526,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -4520,7 +4546,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="18"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -4540,7 +4566,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -4562,7 +4588,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -4584,7 +4610,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="18"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -4600,7 +4626,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -4616,7 +4642,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="18"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -4632,7 +4658,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -4648,7 +4674,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="18"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -4664,7 +4690,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -4680,7 +4706,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -4696,7 +4722,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="18"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -4712,7 +4738,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -4728,7 +4754,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="18"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -4744,7 +4770,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="18"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -4760,7 +4786,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -4776,7 +4802,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="18"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -4792,7 +4818,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -4808,7 +4834,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -4824,7 +4850,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="18"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -4840,7 +4866,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="18"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -4856,7 +4882,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="18"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -4872,7 +4898,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="18"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -4888,7 +4914,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="18"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -4904,7 +4930,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="18"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -4920,7 +4946,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -4936,7 +4962,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="18"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -4952,7 +4978,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4968,7 +4994,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="18"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4984,7 +5010,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="18"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -5000,7 +5026,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -5016,7 +5042,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="18"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -5032,7 +5058,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -5048,7 +5074,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="18"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -5064,7 +5090,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="18"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -5080,7 +5106,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="18"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -5096,7 +5122,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="18"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -5112,7 +5138,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="18"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -5128,7 +5154,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="18"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -5144,7 +5170,7 @@
       <c r="I48" s="14"/>
       <c r="J48" s="18"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -5160,7 +5186,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="18"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -5190,27 +5216,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29566457-B408-4484-B427-3F415D9C9DE3}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.921875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -5242,7 +5268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -5264,7 +5290,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="21"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -5286,7 +5312,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -5308,7 +5334,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -5330,7 +5356,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -5352,7 +5378,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -5374,7 +5400,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5396,7 +5422,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5418,7 +5444,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -5440,7 +5466,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="21"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -5462,7 +5488,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="21"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -5484,7 +5510,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="21"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -5506,7 +5532,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -5528,7 +5554,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -5550,7 +5576,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -5572,7 +5598,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="21"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -5594,7 +5620,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="21"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -5616,7 +5642,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="21"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -5638,7 +5664,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="21"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -5660,7 +5686,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="21"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -5682,7 +5708,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -5704,7 +5730,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -5726,7 +5752,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -5748,7 +5774,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -5770,7 +5796,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="21"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -5792,7 +5818,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -5814,7 +5840,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -5836,7 +5862,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -5858,39 +5884,51 @@
       <c r="I29" s="14"/>
       <c r="J29" s="21"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
+      <c r="C30" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>184</v>
+      </c>
       <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
+      <c r="F30" s="21" t="s">
+        <v>5</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="21"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
+      <c r="C31" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>190</v>
+      </c>
       <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
+      <c r="F31" s="21" t="s">
+        <v>5</v>
+      </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="21"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -5906,7 +5944,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="21"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -5922,7 +5960,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -5938,7 +5976,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="21"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -5954,7 +5992,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -5970,7 +6008,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="21"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -5986,7 +6024,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -6002,7 +6040,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="21"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -6018,7 +6056,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -6034,7 +6072,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -6050,7 +6088,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -6066,7 +6104,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="21"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -6082,7 +6120,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="21"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -6098,7 +6136,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="21"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -6114,7 +6152,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="21"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -6130,7 +6168,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="21"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -6146,7 +6184,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="21"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -6162,7 +6200,7 @@
       <c r="I48" s="14"/>
       <c r="J48" s="21"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -6178,7 +6216,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="21"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -6214,21 +6252,21 @@
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="3" width="20.19921875" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="3" width="20.23046875" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.921875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -6260,7 +6298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -6282,7 +6320,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -6298,7 +6336,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -6314,7 +6352,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="23"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -6330,7 +6368,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="23"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -6346,7 +6384,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -6362,7 +6400,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="23"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -6378,7 +6416,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -6394,7 +6432,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="23"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -6410,7 +6448,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="23"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -6426,7 +6464,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="23"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -6442,7 +6480,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="23"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -6458,7 +6496,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="23"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -6474,7 +6512,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="23"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -6490,7 +6528,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="23"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -6506,7 +6544,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="23"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -6522,7 +6560,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="23"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -6538,7 +6576,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="23"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -6554,7 +6592,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="23"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -6570,7 +6608,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="23"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -6586,7 +6624,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="23"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -6602,7 +6640,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="23"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -6618,7 +6656,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -6634,7 +6672,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="23"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -6650,7 +6688,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="23"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -6666,7 +6704,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="23"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -6682,7 +6720,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="23"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -6698,7 +6736,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="23"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -6714,7 +6752,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="23"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -6730,7 +6768,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -6746,7 +6784,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="23"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -6768,7 +6806,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="25"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -6790,7 +6828,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="25"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -6812,7 +6850,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="25"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -6828,7 +6866,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="25"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -6844,7 +6882,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="25"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -6860,7 +6898,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="25"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -6876,7 +6914,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="25"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -6892,7 +6930,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="25"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -6908,7 +6946,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="25"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -6924,7 +6962,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="25"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -6940,7 +6978,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="25"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -6956,7 +6994,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="25"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -6972,7 +7010,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="25"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -6988,7 +7026,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="25"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -7004,7 +7042,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="25"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -7020,7 +7058,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="25"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -7036,7 +7074,7 @@
       <c r="I48" s="14"/>
       <c r="J48" s="25"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -7052,7 +7090,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="25"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -7068,7 +7106,7 @@
       <c r="I50" s="14"/>
       <c r="J50" s="25"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -7084,7 +7122,7 @@
       <c r="I51" s="14"/>
       <c r="J51" s="25"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -7100,7 +7138,7 @@
       <c r="I52" s="14"/>
       <c r="J52" s="25"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -7116,7 +7154,7 @@
       <c r="I53" s="14"/>
       <c r="J53" s="25"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -7132,7 +7170,7 @@
       <c r="I54" s="14"/>
       <c r="J54" s="25"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -7148,7 +7186,7 @@
       <c r="I55" s="14"/>
       <c r="J55" s="25"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -7164,7 +7202,7 @@
       <c r="I56" s="14"/>
       <c r="J56" s="25"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -7180,7 +7218,7 @@
       <c r="I57" s="14"/>
       <c r="J57" s="25"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -7196,7 +7234,7 @@
       <c r="I58" s="14"/>
       <c r="J58" s="25"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -7212,7 +7250,7 @@
       <c r="I59" s="14"/>
       <c r="J59" s="25"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -7228,7 +7266,7 @@
       <c r="I60" s="14"/>
       <c r="J60" s="25"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -7264,22 +7302,22 @@
       <selection pane="bottomLeft" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.9296875" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" customWidth="1"/>
-    <col min="3" max="3" width="20.19921875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" style="36" customWidth="1"/>
-    <col min="6" max="6" width="74.33203125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="26.59765625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.9296875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="17.9296875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="82.73046875" customWidth="1"/>
-    <col min="11" max="11" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="7.921875" customWidth="1"/>
+    <col min="2" max="2" width="20.23046875" customWidth="1"/>
+    <col min="3" max="3" width="20.23046875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.765625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.23046875" style="36" customWidth="1"/>
+    <col min="6" max="6" width="74.3046875" style="32" customWidth="1"/>
+    <col min="7" max="7" width="26.61328125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.921875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.921875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="82.69140625" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -7311,7 +7349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -7331,7 +7369,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -7351,7 +7389,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -7371,7 +7409,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -7387,7 +7425,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -7403,7 +7441,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="11"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -7419,7 +7457,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -7435,7 +7473,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -7451,7 +7489,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -7467,7 +7505,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -7483,7 +7521,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -7499,7 +7537,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -7515,7 +7553,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -7531,7 +7569,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -7547,7 +7585,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -7563,7 +7601,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -7579,7 +7617,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -7595,7 +7633,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -7611,7 +7649,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -7627,7 +7665,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -7647,7 +7685,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="28"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -7667,7 +7705,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="28"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -7683,7 +7721,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="28"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -7699,7 +7737,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="28"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -7715,7 +7753,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="28"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -7731,7 +7769,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="28"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -7747,7 +7785,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="28"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -7763,7 +7801,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -7779,7 +7817,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="28"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -7795,7 +7833,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="28"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -7811,7 +7849,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="28"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -7827,7 +7865,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="28"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -7843,7 +7881,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="28"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -7859,7 +7897,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="28"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -7875,7 +7913,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="28"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -7891,7 +7929,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="28"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -7907,7 +7945,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="28"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -7923,7 +7961,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="28"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -7939,7 +7977,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="28"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -7955,7 +7993,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="28"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -7982,21 +8020,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E588E3CCEF65154AAAA5938E9E65CE17" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03844ae5e13aa177ebf3507b0751d91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e85ca4a-4ac1-4389-acba-849333013406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb1ad88d086bd6ffd9f20c44ca8152ce" ns2:_="">
     <xsd:import namespace="0e85ca4a-4ac1-4389-acba-849333013406"/>
@@ -8154,15 +8183,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4776DA57-D8F8-44AA-B808-89F6418CE6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECED21D3-74F5-44AF-93F1-3A615F6BB7E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8171,7 +8201,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD09570-86F7-4181-B0EF-3E1223C67D7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8187,4 +8217,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4776DA57-D8F8-44AA-B808-89F6418CE6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>